<commit_message>
Tidying up the functions
</commit_message>
<xml_diff>
--- a/openbb_terminal/portfolio/portfolio_optimization/parameters/OpenBB_Portfolio_Template v1.0.0.xlsx
+++ b/openbb_terminal/portfolio/portfolio_optimization/parameters/OpenBB_Portfolio_Template v1.0.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeroenbouma/Documents/OpenBB Dany/openbb_terminal/portfolio/portfolio_optimization/parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5898A23-796D-F143-B0A0-B9F271B7F0E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D464B0D-2095-574E-A561-6CD942AE1450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-360" windowWidth="38400" windowHeight="21600" xr2:uid="{4E6A10D7-C95B-B048-9E7D-368AD146FDA2}"/>
   </bookViews>
@@ -2845,9 +2845,6 @@
     <xf numFmtId="8" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2864,13 +2861,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -2894,121 +2894,6 @@
     <dxf>
       <font>
         <color theme="0" tint="-0.14996795556505021"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.14996795556505021"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
       </font>
     </dxf>
   </dxfs>
@@ -3370,10 +3255,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D68F2FA-964B-DB41-A4DF-DD4A2F7AD4F5}">
-  <dimension ref="A1:XFD48"/>
+  <dimension ref="A1:XFC48"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="16" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -3382,7 +3267,7 @@
     <col min="2" max="2" width="25.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.83203125" style="3" customWidth="1"/>
     <col min="4" max="4" width="128.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="50" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="49" customWidth="1"/>
     <col min="6" max="16383" width="10.83203125" hidden="1"/>
     <col min="16384" max="16384" width="8.83203125" hidden="1" customWidth="1"/>
   </cols>
@@ -3393,10 +3278,10 @@
       <c r="D1"/>
     </row>
     <row r="2" spans="2:5" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="49" t="s">
+      <c r="C2" s="55" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="49"/>
+      <c r="D2" s="55"/>
     </row>
     <row r="3" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
@@ -3408,12 +3293,12 @@
       <c r="D3" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="50" t="s">
+      <c r="E3" s="49" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="119" x14ac:dyDescent="0.2">
-      <c r="B4" s="52" t="s">
+      <c r="B4" s="51" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="12" t="s">
@@ -3422,39 +3307,39 @@
       <c r="D4" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="51" t="str">
+      <c r="E4" s="50" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B4,CONFIG!$B:$Y,MATCH($C$16,CONFIG!$B$1:$Y$1,0),FALSE),"")</f>
         <v/>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="53" t="s">
+      <c r="B5" s="52" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="E5" s="51" t="str">
+      <c r="E5" s="50" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B5,CONFIG!$B:$Y,MATCH($C$16,CONFIG!$B$1:$Y$1,0),FALSE),"")</f>
         <v/>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B6" s="53" t="s">
+      <c r="B6" s="52" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="E6" s="51" t="str">
+      <c r="E6" s="50" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B6,CONFIG!$B:$Y,MATCH($C$16,CONFIG!$B$1:$Y$1,0),FALSE),"")</f>
         <v/>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B7" s="53" t="s">
+      <c r="B7" s="52" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="8">
@@ -3463,13 +3348,13 @@
       <c r="D7" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="E7" s="51" t="str">
+      <c r="E7" s="50" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B7,CONFIG!$B:$Y,MATCH($C$16,CONFIG!$B$1:$Y$1,0),FALSE),"")</f>
         <v/>
       </c>
     </row>
     <row r="8" spans="2:5" ht="69" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="53" t="s">
+      <c r="B8" s="52" t="s">
         <v>20</v>
       </c>
       <c r="C8" s="8" t="s">
@@ -3478,13 +3363,13 @@
       <c r="D8" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="51" t="str">
+      <c r="E8" s="50" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B8,CONFIG!$B:$Y,MATCH($C$16,CONFIG!$B$1:$Y$1,0),FALSE),"")</f>
         <v/>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="53" t="s">
+      <c r="B9" s="52" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="9">
@@ -3493,13 +3378,13 @@
       <c r="D9" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="E9" s="51" t="str">
+      <c r="E9" s="50" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B9,CONFIG!$B:$Y,MATCH($C$16,CONFIG!$B$1:$Y$1,0),FALSE),"")</f>
         <v/>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="53" t="s">
+      <c r="B10" s="52" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="10">
@@ -3508,13 +3393,13 @@
       <c r="D10" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="E10" s="51" t="str">
+      <c r="E10" s="50" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B10,CONFIG!$B:$Y,MATCH($C$16,CONFIG!$B$1:$Y$1,0),FALSE),"")</f>
         <v/>
       </c>
     </row>
     <row r="11" spans="2:5" ht="136" x14ac:dyDescent="0.2">
-      <c r="B11" s="53" t="s">
+      <c r="B11" s="52" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="8" t="s">
@@ -3523,13 +3408,13 @@
       <c r="D11" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="E11" s="51" t="str">
+      <c r="E11" s="50" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B11,CONFIG!$B:$Y,MATCH($C$16,CONFIG!$B$1:$Y$1,0),FALSE),"")</f>
         <v/>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B12" s="53" t="s">
+      <c r="B12" s="52" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="11">
@@ -3538,13 +3423,13 @@
       <c r="D12" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="E12" s="51" t="str">
+      <c r="E12" s="50" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B12,CONFIG!$B:$Y,MATCH($C$16,CONFIG!$B$1:$Y$1,0),FALSE),"")</f>
         <v/>
       </c>
     </row>
     <row r="13" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="54" t="s">
+      <c r="B13" s="53" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="16">
@@ -3553,13 +3438,13 @@
       <c r="D13" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="E13" s="51" t="str">
+      <c r="E13" s="50" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B13,CONFIG!$B:$Y,MATCH($C$16,CONFIG!$B$1:$Y$1,0),FALSE),"")</f>
         <v/>
       </c>
     </row>
     <row r="14" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E14" s="51" t="str">
+      <c r="E14" s="50" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B14,CONFIG!$B:$Y,MATCH($C$16,CONFIG!$B$1:$Y$1,0),FALSE),"")</f>
         <v/>
       </c>
@@ -3574,13 +3459,13 @@
       <c r="D15" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="51" t="str">
+      <c r="E15" s="50" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B15,CONFIG!$B:$Y,MATCH($C$16,CONFIG!$B$1:$Y$1,0),FALSE),"")</f>
         <v/>
       </c>
     </row>
     <row r="16" spans="2:5" ht="273" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="55" t="s">
+      <c r="B16" s="54" t="s">
         <v>80</v>
       </c>
       <c r="C16" s="22" t="s">
@@ -3589,13 +3474,13 @@
       <c r="D16" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="E16" s="51" t="str">
+      <c r="E16" s="50" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B16,CONFIG!$B:$Y,MATCH($C$16,CONFIG!$B$1:$Y$1,0),FALSE),"")</f>
         <v/>
       </c>
     </row>
     <row r="17" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E17" s="51" t="str">
+      <c r="E17" s="50" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B17,CONFIG!$B:$Y,MATCH($C$16,CONFIG!$B$1:$Y$1,0),FALSE),"")</f>
         <v/>
       </c>
@@ -3610,13 +3495,13 @@
       <c r="D18" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E18" s="51" t="str">
+      <c r="E18" s="50" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B18,CONFIG!$B:$Y,MATCH($C$16,CONFIG!$B$1:$Y$1,0),FALSE),"")</f>
         <v/>
       </c>
     </row>
     <row r="19" spans="2:5" ht="238" x14ac:dyDescent="0.2">
-      <c r="B19" s="52" t="s">
+      <c r="B19" s="51" t="s">
         <v>22</v>
       </c>
       <c r="C19" s="12" t="s">
@@ -3625,13 +3510,13 @@
       <c r="D19" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="E19" s="51" t="str">
+      <c r="E19" s="50" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B19,CONFIG!$B:$Y,MATCH($C$16,CONFIG!$B$1:$Y$1,0),FALSE),"")</f>
         <v>YES</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B20" s="53" t="s">
+      <c r="B20" s="52" t="s">
         <v>12</v>
       </c>
       <c r="C20" s="8">
@@ -3640,13 +3525,13 @@
       <c r="D20" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="E20" s="51" t="str">
+      <c r="E20" s="50" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B20,CONFIG!$B:$Y,MATCH($C$16,CONFIG!$B$1:$Y$1,0),FALSE),"")</f>
         <v>NO</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B21" s="53" t="s">
+      <c r="B21" s="52" t="s">
         <v>13</v>
       </c>
       <c r="C21" s="8">
@@ -3655,13 +3540,13 @@
       <c r="D21" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="E21" s="51" t="str">
+      <c r="E21" s="50" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B21,CONFIG!$B:$Y,MATCH($C$16,CONFIG!$B$1:$Y$1,0),FALSE),"")</f>
         <v>NO</v>
       </c>
     </row>
     <row r="22" spans="2:5" ht="68" x14ac:dyDescent="0.2">
-      <c r="B22" s="53" t="s">
+      <c r="B22" s="52" t="s">
         <v>14</v>
       </c>
       <c r="C22" s="8" t="s">
@@ -3670,13 +3555,13 @@
       <c r="D22" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="E22" s="51" t="str">
+      <c r="E22" s="50" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B22,CONFIG!$B:$Y,MATCH($C$16,CONFIG!$B$1:$Y$1,0),FALSE),"")</f>
         <v>NO</v>
       </c>
     </row>
     <row r="23" spans="2:5" ht="204" x14ac:dyDescent="0.2">
-      <c r="B23" s="53" t="s">
+      <c r="B23" s="52" t="s">
         <v>16</v>
       </c>
       <c r="C23" s="8" t="s">
@@ -3685,13 +3570,13 @@
       <c r="D23" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="E23" s="51" t="str">
+      <c r="E23" s="50" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B23,CONFIG!$B:$Y,MATCH($C$16,CONFIG!$B$1:$Y$1,0),FALSE),"")</f>
         <v>NO</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B24" s="53" t="s">
+      <c r="B24" s="52" t="s">
         <v>46</v>
       </c>
       <c r="C24" s="9">
@@ -3700,13 +3585,13 @@
       <c r="D24" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="E24" s="51" t="str">
+      <c r="E24" s="50" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B24,CONFIG!$B:$Y,MATCH($C$16,CONFIG!$B$1:$Y$1,0),FALSE),"")</f>
         <v>NO</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B25" s="53" t="s">
+      <c r="B25" s="52" t="s">
         <v>17</v>
       </c>
       <c r="C25" s="8">
@@ -3715,13 +3600,13 @@
       <c r="D25" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="E25" s="51" t="str">
+      <c r="E25" s="50" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B25,CONFIG!$B:$Y,MATCH($C$16,CONFIG!$B$1:$Y$1,0),FALSE),"")</f>
         <v>YES</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B26" s="53" t="s">
+      <c r="B26" s="52" t="s">
         <v>18</v>
       </c>
       <c r="C26" s="8">
@@ -3730,13 +3615,13 @@
       <c r="D26" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="E26" s="51" t="str">
+      <c r="E26" s="50" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B26,CONFIG!$B:$Y,MATCH($C$16,CONFIG!$B$1:$Y$1,0),FALSE),"")</f>
         <v>YES</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B27" s="53" t="s">
+      <c r="B27" s="52" t="s">
         <v>19</v>
       </c>
       <c r="C27" s="8">
@@ -3745,13 +3630,13 @@
       <c r="D27" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="E27" s="51" t="str">
+      <c r="E27" s="50" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B27,CONFIG!$B:$Y,MATCH($C$16,CONFIG!$B$1:$Y$1,0),FALSE),"")</f>
         <v>NO</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B28" s="53" t="s">
+      <c r="B28" s="52" t="s">
         <v>144</v>
       </c>
       <c r="C28" s="8">
@@ -3760,13 +3645,13 @@
       <c r="D28" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="E28" s="51" t="str">
+      <c r="E28" s="50" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B28,CONFIG!$B:$Y,MATCH($C$16,CONFIG!$B$1:$Y$1,0),FALSE),"")</f>
         <v>YES</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B29" s="53" t="s">
+      <c r="B29" s="52" t="s">
         <v>145</v>
       </c>
       <c r="C29" s="8">
@@ -3775,13 +3660,13 @@
       <c r="D29" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="E29" s="51" t="str">
+      <c r="E29" s="50" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B29,CONFIG!$B:$Y,MATCH($C$16,CONFIG!$B$1:$Y$1,0),FALSE),"")</f>
         <v>YES</v>
       </c>
     </row>
     <row r="30" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="54" t="s">
+      <c r="B30" s="53" t="s">
         <v>146</v>
       </c>
       <c r="C30" s="18">
@@ -3790,14 +3675,14 @@
       <c r="D30" s="17" t="s">
         <v>148</v>
       </c>
-      <c r="E30" s="51" t="str">
+      <c r="E30" s="50" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B30,CONFIG!$B:$Y,MATCH($C$16,CONFIG!$B$1:$Y$1,0),FALSE),"")</f>
         <v>YES</v>
       </c>
     </row>
     <row r="31" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B31" s="4"/>
-      <c r="E31" s="51" t="str">
+      <c r="E31" s="50" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B31,CONFIG!$B:$Y,MATCH($C$16,CONFIG!$B$1:$Y$1,0),FALSE),"")</f>
         <v/>
       </c>
@@ -3812,26 +3697,26 @@
       <c r="D32" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E32" s="51" t="str">
+      <c r="E32" s="50" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B32,CONFIG!$B:$Y,MATCH($C$16,CONFIG!$B$1:$Y$1,0),FALSE),"")</f>
         <v/>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B33" s="52" t="s">
+      <c r="B33" s="51" t="s">
         <v>23</v>
       </c>
       <c r="C33" s="12"/>
       <c r="D33" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="E33" s="51" t="str">
+      <c r="E33" s="50" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B33,CONFIG!$B:$Y,MATCH($C$16,CONFIG!$B$1:$Y$1,0),FALSE),"")</f>
         <v>NO</v>
       </c>
     </row>
     <row r="34" spans="2:5" ht="68" x14ac:dyDescent="0.2">
-      <c r="B34" s="53" t="s">
+      <c r="B34" s="52" t="s">
         <v>24</v>
       </c>
       <c r="C34" s="8" t="s">
@@ -3840,13 +3725,13 @@
       <c r="D34" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E34" s="51" t="str">
+      <c r="E34" s="50" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B34,CONFIG!$B:$Y,MATCH($C$16,CONFIG!$B$1:$Y$1,0),FALSE),"")</f>
         <v>NO</v>
       </c>
     </row>
     <row r="35" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="54" t="s">
+      <c r="B35" s="53" t="s">
         <v>25</v>
       </c>
       <c r="C35" s="18">
@@ -3855,13 +3740,13 @@
       <c r="D35" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="E35" s="51" t="str">
+      <c r="E35" s="50" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B35,CONFIG!$B:$Y,MATCH($C$16,CONFIG!$B$1:$Y$1,0),FALSE),"")</f>
         <v>NO</v>
       </c>
     </row>
     <row r="36" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E36" s="51" t="str">
+      <c r="E36" s="50" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B36,CONFIG!$B:$Y,MATCH($C$16,CONFIG!$B$1:$Y$1,0),FALSE),"")</f>
         <v/>
       </c>
@@ -3876,13 +3761,13 @@
       <c r="D37" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E37" s="51" t="str">
+      <c r="E37" s="50" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B37,CONFIG!$B:$Y,MATCH($C$16,CONFIG!$B$1:$Y$1,0),FALSE),"")</f>
         <v/>
       </c>
     </row>
     <row r="38" spans="2:5" ht="136" x14ac:dyDescent="0.2">
-      <c r="B38" s="52" t="s">
+      <c r="B38" s="51" t="s">
         <v>26</v>
       </c>
       <c r="C38" s="12" t="s">
@@ -3891,13 +3776,13 @@
       <c r="D38" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="E38" s="51" t="str">
+      <c r="E38" s="50" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B38,CONFIG!$B:$Y,MATCH($C$16,CONFIG!$B$1:$Y$1,0),FALSE),"")</f>
         <v>NO</v>
       </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B39" s="53" t="s">
+      <c r="B39" s="52" t="s">
         <v>129</v>
       </c>
       <c r="C39" s="8">
@@ -3906,13 +3791,13 @@
       <c r="D39" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E39" s="51" t="str">
+      <c r="E39" s="50" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B39,CONFIG!$B:$Y,MATCH($C$16,CONFIG!$B$1:$Y$1,0),FALSE),"")</f>
         <v>NO</v>
       </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B40" s="53" t="s">
+      <c r="B40" s="52" t="s">
         <v>29</v>
       </c>
       <c r="C40" s="9">
@@ -3922,13 +3807,13 @@
       <c r="D40" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="E40" s="51" t="str">
+      <c r="E40" s="50" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B40,CONFIG!$B:$Y,MATCH($C$16,CONFIG!$B$1:$Y$1,0),FALSE),"")</f>
         <v>NO</v>
       </c>
     </row>
     <row r="41" spans="2:5" ht="136" x14ac:dyDescent="0.2">
-      <c r="B41" s="53" t="s">
+      <c r="B41" s="52" t="s">
         <v>31</v>
       </c>
       <c r="C41" s="8" t="s">
@@ -3937,26 +3822,29 @@
       <c r="D41" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="E41" s="51" t="str">
+      <c r="E41" s="50" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B41,CONFIG!$B:$Y,MATCH($C$16,CONFIG!$B$1:$Y$1,0),FALSE),"")</f>
         <v>NO</v>
       </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B42" s="53" t="s">
+      <c r="B42" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="C42" s="8"/>
+      <c r="C42" s="8">
+        <f>C43</f>
+        <v>10</v>
+      </c>
       <c r="D42" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="E42" s="51" t="str">
+      <c r="E42" s="50" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B42,CONFIG!$B:$Y,MATCH($C$16,CONFIG!$B$1:$Y$1,0),FALSE),"")</f>
         <v>NO</v>
       </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B43" s="53" t="s">
+      <c r="B43" s="52" t="s">
         <v>34</v>
       </c>
       <c r="C43" s="8">
@@ -3965,13 +3853,13 @@
       <c r="D43" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="E43" s="51" t="str">
+      <c r="E43" s="50" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B43,CONFIG!$B:$Y,MATCH($C$16,CONFIG!$B$1:$Y$1,0),FALSE),"")</f>
         <v>NO</v>
       </c>
     </row>
     <row r="44" spans="2:5" ht="102" x14ac:dyDescent="0.2">
-      <c r="B44" s="53" t="s">
+      <c r="B44" s="52" t="s">
         <v>37</v>
       </c>
       <c r="C44" s="8" t="s">
@@ -3980,13 +3868,13 @@
       <c r="D44" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="E44" s="51" t="str">
+      <c r="E44" s="50" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B44,CONFIG!$B:$Y,MATCH($C$16,CONFIG!$B$1:$Y$1,0),FALSE),"")</f>
         <v>NO</v>
       </c>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B45" s="53" t="s">
+      <c r="B45" s="52" t="s">
         <v>39</v>
       </c>
       <c r="C45" s="9">
@@ -3995,13 +3883,13 @@
       <c r="D45" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="E45" s="51" t="str">
+      <c r="E45" s="50" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B45,CONFIG!$B:$Y,MATCH($C$16,CONFIG!$B$1:$Y$1,0),FALSE),"")</f>
         <v>NO</v>
       </c>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B46" s="53" t="s">
+      <c r="B46" s="52" t="s">
         <v>41</v>
       </c>
       <c r="C46" s="8">
@@ -4010,13 +3898,13 @@
       <c r="D46" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="E46" s="51" t="str">
+      <c r="E46" s="50" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B46,CONFIG!$B:$Y,MATCH($C$16,CONFIG!$B$1:$Y$1,0),FALSE),"")</f>
         <v>NO</v>
       </c>
     </row>
     <row r="47" spans="2:5" ht="86" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="54" t="s">
+      <c r="B47" s="53" t="s">
         <v>43</v>
       </c>
       <c r="C47" s="18" t="s">
@@ -4025,7 +3913,7 @@
       <c r="D47" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="E47" s="51" t="str">
+      <c r="E47" s="50" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B47,CONFIG!$B:$Y,MATCH($C$16,CONFIG!$B$1:$Y$1,0),FALSE),"")</f>
         <v>NO</v>
       </c>

</xml_diff>